<commit_message>
Sequences with multiple PPO domains
</commit_message>
<xml_diff>
--- a/data/proteome-tree/class-representatives.xlsx
+++ b/data/proteome-tree/class-representatives.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idamei/polyphenol-oxidases/data/proteome-tree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C081940-35CF-9847-8A06-BEFF573BD654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D820B613-F968-BC4F-9704-57A81D9C8915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{F5F2D1A1-B58F-E84D-BA53-6173843C03DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="753">
   <si>
     <t>UP000077248</t>
   </si>
@@ -1895,63 +1895,6 @@
     <t>Nannochloropsis gaditana</t>
   </si>
   <si>
-    <t>UP000054560</t>
-  </si>
-  <si>
-    <t>Ichthyosporea</t>
-  </si>
-  <si>
-    <t>Ichthyophonida</t>
-  </si>
-  <si>
-    <t>Sphaeroforma</t>
-  </si>
-  <si>
-    <t>Sphaeroforma arctica</t>
-  </si>
-  <si>
-    <t>Sphaeroforma arctica JP610</t>
-  </si>
-  <si>
-    <t>UP000002729</t>
-  </si>
-  <si>
-    <t>Pelagophyceae</t>
-  </si>
-  <si>
-    <t>Pelagomonadales</t>
-  </si>
-  <si>
-    <t>Aureococcus</t>
-  </si>
-  <si>
-    <t>Aureococcus anophagefferens</t>
-  </si>
-  <si>
-    <t>Aureococcus anophagefferens (Harmful bloom alga)</t>
-  </si>
-  <si>
-    <t>UP000002630</t>
-  </si>
-  <si>
-    <t>Phaeophyceae</t>
-  </si>
-  <si>
-    <t>Ectocarpales</t>
-  </si>
-  <si>
-    <t>Ectocarpaceae</t>
-  </si>
-  <si>
-    <t>Ectocarpus</t>
-  </si>
-  <si>
-    <t>Ectocarpus siliculosus</t>
-  </si>
-  <si>
-    <t>Ectocarpus siliculosus (Brown alga) (Conferva siliculosa)</t>
-  </si>
-  <si>
     <t>UP000664859</t>
   </si>
   <si>
@@ -2039,27 +1982,6 @@
     <t>Gracilariopsis chorda</t>
   </si>
   <si>
-    <t>UP000452269</t>
-  </si>
-  <si>
-    <t>Thaumarchaeota</t>
-  </si>
-  <si>
-    <t>Nitrososphaeria</t>
-  </si>
-  <si>
-    <t>Nitrososphaerales</t>
-  </si>
-  <si>
-    <t>Nitrososphaeraceae</t>
-  </si>
-  <si>
-    <t>Nitrososphaeraceae archaeon</t>
-  </si>
-  <si>
-    <t>thaumarchaeota_odb10</t>
-  </si>
-  <si>
     <t>UP000321577</t>
   </si>
   <si>
@@ -2169,27 +2091,6 @@
   </si>
   <si>
     <t>Marchantia polymorpha subsp. ruderalis</t>
-  </si>
-  <si>
-    <t>UP000886520</t>
-  </si>
-  <si>
-    <t>Polypodiopsida</t>
-  </si>
-  <si>
-    <t>Polypodiales</t>
-  </si>
-  <si>
-    <t>Pteridaceae</t>
-  </si>
-  <si>
-    <t>Adiantum</t>
-  </si>
-  <si>
-    <t>Adiantum capillus-veneris</t>
-  </si>
-  <si>
-    <t>Adiantum capillus-veneris (Maidenhair fern)</t>
   </si>
   <si>
     <t>UP000003163</t>
@@ -2453,27 +2354,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2814,86 +2704,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55AD071-326A-564C-9452-BA0C45FD02D7}">
-  <dimension ref="A1:X103"/>
+  <dimension ref="A1:X97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>759</v>
+        <v>726</v>
       </c>
       <c r="B1" t="s">
-        <v>760</v>
+        <v>727</v>
       </c>
       <c r="C1" t="s">
-        <v>761</v>
+        <v>728</v>
       </c>
       <c r="D1" t="s">
-        <v>762</v>
+        <v>729</v>
       </c>
       <c r="E1" t="s">
-        <v>763</v>
+        <v>730</v>
       </c>
       <c r="F1" t="s">
-        <v>764</v>
+        <v>731</v>
       </c>
       <c r="G1" t="s">
-        <v>765</v>
+        <v>732</v>
       </c>
       <c r="H1" t="s">
-        <v>766</v>
+        <v>733</v>
       </c>
       <c r="I1" t="s">
-        <v>767</v>
+        <v>734</v>
       </c>
       <c r="J1" t="s">
-        <v>768</v>
+        <v>735</v>
       </c>
       <c r="K1" t="s">
-        <v>769</v>
+        <v>736</v>
       </c>
       <c r="L1" t="s">
-        <v>770</v>
+        <v>737</v>
       </c>
       <c r="M1" t="s">
-        <v>771</v>
+        <v>738</v>
       </c>
       <c r="N1" t="s">
-        <v>772</v>
+        <v>739</v>
       </c>
       <c r="O1" t="s">
-        <v>773</v>
+        <v>740</v>
       </c>
       <c r="P1" t="s">
-        <v>774</v>
+        <v>741</v>
       </c>
       <c r="Q1" t="s">
-        <v>775</v>
+        <v>742</v>
       </c>
       <c r="R1" t="s">
-        <v>776</v>
+        <v>743</v>
       </c>
       <c r="S1" t="s">
-        <v>777</v>
+        <v>744</v>
       </c>
       <c r="T1" t="s">
-        <v>778</v>
+        <v>745</v>
       </c>
       <c r="U1" t="s">
-        <v>779</v>
+        <v>746</v>
       </c>
       <c r="V1" t="s">
-        <v>780</v>
+        <v>747</v>
       </c>
       <c r="W1" t="s">
-        <v>781</v>
+        <v>748</v>
       </c>
       <c r="X1" t="s">
-        <v>782</v>
+        <v>749</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3046,7 +2939,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>783</v>
+        <v>750</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -3064,10 +2957,10 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>784</v>
+        <v>751</v>
       </c>
       <c r="H4" t="s">
-        <v>785</v>
+        <v>752</v>
       </c>
       <c r="I4">
         <v>4</v>
@@ -3076,7 +2969,7 @@
         <v>1670608</v>
       </c>
       <c r="K4" t="s">
-        <v>785</v>
+        <v>752</v>
       </c>
       <c r="L4">
         <v>1517</v>
@@ -8833,46 +8726,46 @@
         <v>621</v>
       </c>
       <c r="F82" t="s">
-        <v>83</v>
+        <v>622</v>
       </c>
       <c r="G82" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="H82" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="I82">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J82">
-        <v>667725</v>
+        <v>303371</v>
       </c>
       <c r="K82" t="s">
         <v>624</v>
       </c>
       <c r="L82">
-        <v>161</v>
+        <v>93</v>
       </c>
       <c r="M82">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="N82">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O82">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="P82">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="Q82">
-        <v>255</v>
+        <v>100</v>
       </c>
       <c r="R82" t="s">
-        <v>251</v>
+        <v>210</v>
       </c>
       <c r="S82">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="T82">
         <v>0</v>
@@ -8898,55 +8791,55 @@
         <v>83</v>
       </c>
       <c r="C83" t="s">
-        <v>83</v>
+        <v>626</v>
       </c>
       <c r="D83" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E83" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F83" t="s">
-        <v>83</v>
+        <v>629</v>
       </c>
       <c r="G83" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="H83" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="I83">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="J83">
-        <v>44056</v>
+        <v>886293</v>
       </c>
       <c r="K83" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="L83">
-        <v>85</v>
+        <v>568</v>
       </c>
       <c r="M83">
-        <v>82</v>
+        <v>562</v>
       </c>
       <c r="N83">
+        <v>6</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="P83">
         <v>3</v>
       </c>
-      <c r="O83">
-        <v>10</v>
-      </c>
-      <c r="P83">
-        <v>5</v>
-      </c>
       <c r="Q83">
-        <v>100</v>
+        <v>571</v>
       </c>
       <c r="R83" t="s">
-        <v>210</v>
+        <v>633</v>
       </c>
       <c r="S83">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="T83">
         <v>0</v>
@@ -8966,61 +8859,61 @@
     </row>
     <row r="84" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="B84" t="s">
         <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>83</v>
+        <v>635</v>
       </c>
       <c r="D84" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="E84" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="F84" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="G84" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="H84" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="I84">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="J84">
-        <v>2880</v>
+        <v>130081</v>
       </c>
       <c r="K84" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="L84">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="M84">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="N84">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="O84">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="P84">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="Q84">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="R84" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
       <c r="S84">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="T84">
         <v>0</v>
@@ -9040,61 +8933,61 @@
     </row>
     <row r="85" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B85" t="s">
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>83</v>
+        <v>635</v>
       </c>
       <c r="D85" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="E85" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="F85" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="G85" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="H85" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="I85">
         <v>3</v>
       </c>
       <c r="J85">
-        <v>303371</v>
+        <v>448386</v>
       </c>
       <c r="K85" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="L85">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="M85">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="N85">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O85">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="P85">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="Q85">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="R85" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
       <c r="S85">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="T85">
         <v>0</v>
@@ -9114,64 +9007,64 @@
     </row>
     <row r="86" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="B86" t="s">
         <v>83</v>
       </c>
       <c r="C86" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="D86" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="E86" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="F86" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c r="G86" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="H86" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="I86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J86">
-        <v>886293</v>
+        <v>748831</v>
       </c>
       <c r="K86" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="L86">
-        <v>568</v>
+        <v>461</v>
       </c>
       <c r="M86">
-        <v>562</v>
+        <v>456</v>
       </c>
       <c r="N86">
+        <v>5</v>
+      </c>
+      <c r="O86">
+        <v>4</v>
+      </c>
+      <c r="P86">
         <v>6</v>
       </c>
-      <c r="O86">
-        <v>0</v>
-      </c>
-      <c r="P86">
-        <v>3</v>
-      </c>
       <c r="Q86">
-        <v>571</v>
+        <v>471</v>
       </c>
       <c r="R86" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="S86">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T86">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="U86">
         <v>0</v>
@@ -9183,66 +9076,66 @@
         <v>0</v>
       </c>
       <c r="X86" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="B87" t="s">
-        <v>83</v>
+        <v>253</v>
       </c>
       <c r="C87" t="s">
-        <v>654</v>
+        <v>271</v>
       </c>
       <c r="D87" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="E87" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="F87" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="G87" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="H87" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="I87">
         <v>1</v>
       </c>
       <c r="J87">
-        <v>130081</v>
+        <v>554065</v>
       </c>
       <c r="K87" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="L87">
-        <v>199</v>
+        <v>1411</v>
       </c>
       <c r="M87">
-        <v>173</v>
+        <v>1396</v>
       </c>
       <c r="N87">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="O87">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="P87">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="Q87">
-        <v>255</v>
+        <v>1519</v>
       </c>
       <c r="R87" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="S87">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="T87">
         <v>0</v>
@@ -9262,61 +9155,61 @@
     </row>
     <row r="88" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B88" t="s">
+        <v>253</v>
+      </c>
+      <c r="C88" t="s">
+        <v>254</v>
+      </c>
+      <c r="D88" t="s">
+        <v>664</v>
+      </c>
+      <c r="E88" t="s">
+        <v>665</v>
+      </c>
+      <c r="F88" t="s">
+        <v>666</v>
+      </c>
+      <c r="G88" t="s">
+        <v>667</v>
+      </c>
+      <c r="H88" t="s">
+        <v>668</v>
+      </c>
+      <c r="I88">
+        <v>16</v>
+      </c>
+      <c r="J88">
+        <v>69332</v>
+      </c>
+      <c r="K88" t="s">
+        <v>669</v>
+      </c>
+      <c r="L88">
+        <v>307</v>
+      </c>
+      <c r="M88">
+        <v>278</v>
+      </c>
+      <c r="N88">
+        <v>29</v>
+      </c>
+      <c r="O88">
+        <v>49</v>
+      </c>
+      <c r="P88">
+        <v>69</v>
+      </c>
+      <c r="Q88">
+        <v>425</v>
+      </c>
+      <c r="R88" t="s">
+        <v>670</v>
+      </c>
+      <c r="S88">
         <v>83</v>
-      </c>
-      <c r="C88" t="s">
-        <v>654</v>
-      </c>
-      <c r="D88" t="s">
-        <v>662</v>
-      </c>
-      <c r="E88" t="s">
-        <v>663</v>
-      </c>
-      <c r="F88" t="s">
-        <v>664</v>
-      </c>
-      <c r="G88" t="s">
-        <v>665</v>
-      </c>
-      <c r="H88" t="s">
-        <v>666</v>
-      </c>
-      <c r="I88">
-        <v>3</v>
-      </c>
-      <c r="J88">
-        <v>448386</v>
-      </c>
-      <c r="K88" t="s">
-        <v>666</v>
-      </c>
-      <c r="L88">
-        <v>206</v>
-      </c>
-      <c r="M88">
-        <v>201</v>
-      </c>
-      <c r="N88">
-        <v>5</v>
-      </c>
-      <c r="O88">
-        <v>13</v>
-      </c>
-      <c r="P88">
-        <v>36</v>
-      </c>
-      <c r="Q88">
-        <v>255</v>
-      </c>
-      <c r="R88" t="s">
-        <v>251</v>
-      </c>
-      <c r="S88">
-        <v>85</v>
       </c>
       <c r="T88">
         <v>0</v>
@@ -9336,61 +9229,61 @@
     </row>
     <row r="89" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>253</v>
       </c>
       <c r="C89" t="s">
-        <v>668</v>
+        <v>254</v>
       </c>
       <c r="D89" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="E89" t="s">
+        <v>673</v>
+      </c>
+      <c r="F89" t="s">
+        <v>674</v>
+      </c>
+      <c r="G89" t="s">
+        <v>675</v>
+      </c>
+      <c r="H89" t="s">
+        <v>676</v>
+      </c>
+      <c r="I89">
+        <v>6</v>
+      </c>
+      <c r="J89">
+        <v>105231</v>
+      </c>
+      <c r="K89" t="s">
+        <v>677</v>
+      </c>
+      <c r="L89">
+        <v>412</v>
+      </c>
+      <c r="M89">
+        <v>410</v>
+      </c>
+      <c r="N89">
+        <v>2</v>
+      </c>
+      <c r="O89">
+        <v>8</v>
+      </c>
+      <c r="P89">
+        <v>5</v>
+      </c>
+      <c r="Q89">
+        <v>425</v>
+      </c>
+      <c r="R89" t="s">
         <v>670</v>
       </c>
-      <c r="F89" t="s">
-        <v>671</v>
-      </c>
-      <c r="G89" t="s">
-        <v>83</v>
-      </c>
-      <c r="H89" t="s">
-        <v>672</v>
-      </c>
-      <c r="I89">
-        <v>2</v>
-      </c>
-      <c r="J89">
-        <v>2169593</v>
-      </c>
-      <c r="K89" t="s">
-        <v>672</v>
-      </c>
-      <c r="L89">
-        <v>613</v>
-      </c>
-      <c r="M89">
-        <v>600</v>
-      </c>
-      <c r="N89">
-        <v>13</v>
-      </c>
-      <c r="O89">
-        <v>7</v>
-      </c>
-      <c r="P89">
-        <v>102</v>
-      </c>
-      <c r="Q89">
-        <v>722</v>
-      </c>
-      <c r="R89" t="s">
-        <v>673</v>
-      </c>
       <c r="S89">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="T89">
         <v>0</v>
@@ -9410,132 +9303,132 @@
     </row>
     <row r="90" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="B90" t="s">
+        <v>253</v>
+      </c>
+      <c r="C90" t="s">
+        <v>254</v>
+      </c>
+      <c r="D90" t="s">
+        <v>679</v>
+      </c>
+      <c r="E90" t="s">
+        <v>680</v>
+      </c>
+      <c r="F90" t="s">
+        <v>681</v>
+      </c>
+      <c r="G90" t="s">
+        <v>682</v>
+      </c>
+      <c r="H90" t="s">
+        <v>683</v>
+      </c>
+      <c r="I90">
+        <v>34</v>
+      </c>
+      <c r="J90">
+        <v>1480154</v>
+      </c>
+      <c r="K90" t="s">
+        <v>684</v>
+      </c>
+      <c r="L90">
+        <v>1290</v>
+      </c>
+      <c r="M90">
+        <v>1273</v>
+      </c>
+      <c r="N90">
+        <v>17</v>
+      </c>
+      <c r="O90">
+        <v>79</v>
+      </c>
+      <c r="P90">
+        <v>245</v>
+      </c>
+      <c r="Q90">
+        <v>1614</v>
+      </c>
+      <c r="R90" t="s">
+        <v>269</v>
+      </c>
+      <c r="S90">
+        <v>84</v>
+      </c>
+      <c r="T90">
+        <v>0</v>
+      </c>
+      <c r="U90">
+        <v>0</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+      <c r="W90">
+        <v>0</v>
+      </c>
+      <c r="X90" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>685</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>686</v>
+      </c>
+      <c r="D91" t="s">
+        <v>687</v>
+      </c>
+      <c r="E91" t="s">
         <v>83</v>
       </c>
-      <c r="C90" t="s">
-        <v>675</v>
-      </c>
-      <c r="D90" t="s">
-        <v>676</v>
-      </c>
-      <c r="E90" t="s">
-        <v>677</v>
-      </c>
-      <c r="F90" t="s">
-        <v>678</v>
-      </c>
-      <c r="G90" t="s">
-        <v>679</v>
-      </c>
-      <c r="H90" t="s">
-        <v>680</v>
-      </c>
-      <c r="I90">
-        <v>2</v>
-      </c>
-      <c r="J90">
-        <v>748831</v>
-      </c>
-      <c r="K90" t="s">
-        <v>680</v>
-      </c>
-      <c r="L90">
-        <v>461</v>
-      </c>
-      <c r="M90">
-        <v>456</v>
-      </c>
-      <c r="N90">
-        <v>5</v>
-      </c>
-      <c r="O90">
-        <v>4</v>
-      </c>
-      <c r="P90">
-        <v>6</v>
-      </c>
-      <c r="Q90">
-        <v>471</v>
-      </c>
-      <c r="R90" t="s">
-        <v>681</v>
-      </c>
-      <c r="S90">
-        <v>98</v>
-      </c>
-      <c r="T90">
-        <v>59</v>
-      </c>
-      <c r="U90">
-        <v>0</v>
-      </c>
-      <c r="V90">
-        <v>0</v>
-      </c>
-      <c r="W90">
-        <v>0</v>
-      </c>
-      <c r="X90" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="91" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>682</v>
-      </c>
-      <c r="B91" t="s">
-        <v>253</v>
-      </c>
-      <c r="C91" t="s">
-        <v>271</v>
-      </c>
-      <c r="D91" t="s">
-        <v>683</v>
-      </c>
-      <c r="E91" t="s">
-        <v>684</v>
-      </c>
       <c r="F91" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="G91" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="H91" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="I91">
         <v>1</v>
       </c>
       <c r="J91">
-        <v>554065</v>
+        <v>1003232</v>
       </c>
       <c r="K91" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="L91">
-        <v>1411</v>
+        <v>544</v>
       </c>
       <c r="M91">
-        <v>1396</v>
+        <v>540</v>
       </c>
       <c r="N91">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="O91">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="P91">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="Q91">
-        <v>1519</v>
+        <v>600</v>
       </c>
       <c r="R91" t="s">
-        <v>278</v>
+        <v>692</v>
       </c>
       <c r="S91">
         <v>95</v>
@@ -9556,63 +9449,63 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="B92" t="s">
-        <v>253</v>
+        <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>254</v>
+        <v>98</v>
       </c>
       <c r="D92" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="E92" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="F92" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="G92" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="H92" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="I92">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J92">
-        <v>69332</v>
+        <v>8496</v>
       </c>
       <c r="K92" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="L92">
-        <v>307</v>
+        <v>6524</v>
       </c>
       <c r="M92">
-        <v>278</v>
+        <v>4968</v>
       </c>
       <c r="N92">
-        <v>29</v>
+        <v>1556</v>
       </c>
       <c r="O92">
-        <v>49</v>
+        <v>318</v>
       </c>
       <c r="P92">
-        <v>69</v>
+        <v>638</v>
       </c>
       <c r="Q92">
-        <v>425</v>
+        <v>7480</v>
       </c>
       <c r="R92" t="s">
-        <v>696</v>
+        <v>137</v>
       </c>
       <c r="S92">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="T92">
         <v>0</v>
@@ -9630,211 +9523,211 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="B93" t="s">
-        <v>253</v>
+        <v>83</v>
       </c>
       <c r="C93" t="s">
-        <v>254</v>
-      </c>
-      <c r="D93" t="s">
-        <v>698</v>
+        <v>701</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>702</v>
       </c>
       <c r="E93" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="F93" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="G93" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="H93" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="I93">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J93">
-        <v>105231</v>
+        <v>2005467</v>
       </c>
       <c r="K93" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="L93">
-        <v>412</v>
+        <v>1886</v>
       </c>
       <c r="M93">
-        <v>410</v>
+        <v>1879</v>
       </c>
       <c r="N93">
+        <v>7</v>
+      </c>
+      <c r="O93">
         <v>2</v>
       </c>
-      <c r="O93">
-        <v>8</v>
-      </c>
       <c r="P93">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="Q93">
-        <v>425</v>
+        <v>1899</v>
       </c>
       <c r="R93" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="S93">
+        <v>99</v>
+      </c>
+      <c r="T93">
+        <v>50</v>
+      </c>
+      <c r="U93">
+        <v>0</v>
+      </c>
+      <c r="V93">
+        <v>0</v>
+      </c>
+      <c r="W93">
+        <v>0</v>
+      </c>
+      <c r="X93" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>203</v>
+      </c>
+      <c r="B94" t="s">
+        <v>83</v>
+      </c>
+      <c r="C94" t="s">
+        <v>204</v>
+      </c>
+      <c r="D94" t="s">
+        <v>205</v>
+      </c>
+      <c r="E94" t="s">
+        <v>205</v>
+      </c>
+      <c r="F94" t="s">
+        <v>206</v>
+      </c>
+      <c r="G94" t="s">
+        <v>207</v>
+      </c>
+      <c r="H94" t="s">
+        <v>208</v>
+      </c>
+      <c r="I94">
+        <v>14</v>
+      </c>
+      <c r="J94">
+        <v>403677</v>
+      </c>
+      <c r="K94" t="s">
+        <v>209</v>
+      </c>
+      <c r="L94">
+        <v>100</v>
+      </c>
+      <c r="M94">
+        <v>99</v>
+      </c>
+      <c r="N94">
+        <v>1</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>100</v>
+      </c>
+      <c r="R94" t="s">
+        <v>210</v>
+      </c>
+      <c r="S94">
+        <v>100</v>
+      </c>
+      <c r="T94">
+        <v>46</v>
+      </c>
+      <c r="U94">
+        <v>0</v>
+      </c>
+      <c r="V94">
+        <v>0</v>
+      </c>
+      <c r="W94">
+        <v>0</v>
+      </c>
+      <c r="X94" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>709</v>
+      </c>
+      <c r="B95" t="s">
+        <v>83</v>
+      </c>
+      <c r="C95" t="s">
+        <v>204</v>
+      </c>
+      <c r="D95" t="s">
+        <v>710</v>
+      </c>
+      <c r="E95" t="s">
+        <v>710</v>
+      </c>
+      <c r="F95" t="s">
+        <v>711</v>
+      </c>
+      <c r="G95" t="s">
+        <v>712</v>
+      </c>
+      <c r="H95" t="s">
+        <v>713</v>
+      </c>
+      <c r="I95">
+        <v>4</v>
+      </c>
+      <c r="J95">
+        <v>65357</v>
+      </c>
+      <c r="K95" t="s">
+        <v>713</v>
+      </c>
+      <c r="L95">
         <v>98</v>
       </c>
-      <c r="T93">
-        <v>0</v>
-      </c>
-      <c r="U93">
-        <v>0</v>
-      </c>
-      <c r="V93">
-        <v>0</v>
-      </c>
-      <c r="W93">
-        <v>0</v>
-      </c>
-      <c r="X93" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="94" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>704</v>
-      </c>
-      <c r="B94" t="s">
-        <v>253</v>
-      </c>
-      <c r="C94" t="s">
-        <v>254</v>
-      </c>
-      <c r="D94" t="s">
-        <v>705</v>
-      </c>
-      <c r="E94" t="s">
-        <v>706</v>
-      </c>
-      <c r="F94" t="s">
-        <v>707</v>
-      </c>
-      <c r="G94" t="s">
-        <v>708</v>
-      </c>
-      <c r="H94" t="s">
-        <v>709</v>
-      </c>
-      <c r="I94">
-        <v>34</v>
-      </c>
-      <c r="J94">
-        <v>1480154</v>
-      </c>
-      <c r="K94" t="s">
-        <v>710</v>
-      </c>
-      <c r="L94">
-        <v>1290</v>
-      </c>
-      <c r="M94">
-        <v>1273</v>
-      </c>
-      <c r="N94">
-        <v>17</v>
-      </c>
-      <c r="O94">
-        <v>79</v>
-      </c>
-      <c r="P94">
-        <v>245</v>
-      </c>
-      <c r="Q94">
-        <v>1614</v>
-      </c>
-      <c r="R94" t="s">
-        <v>269</v>
-      </c>
-      <c r="S94">
-        <v>84</v>
-      </c>
-      <c r="T94">
-        <v>0</v>
-      </c>
-      <c r="U94">
-        <v>0</v>
-      </c>
-      <c r="V94">
-        <v>0</v>
-      </c>
-      <c r="W94">
-        <v>0</v>
-      </c>
-      <c r="X94" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>711</v>
-      </c>
-      <c r="B95" t="s">
-        <v>253</v>
-      </c>
-      <c r="C95" t="s">
-        <v>254</v>
-      </c>
-      <c r="D95" t="s">
-        <v>712</v>
-      </c>
-      <c r="E95" t="s">
-        <v>713</v>
-      </c>
-      <c r="F95" t="s">
-        <v>714</v>
-      </c>
-      <c r="G95" t="s">
-        <v>715</v>
-      </c>
-      <c r="H95" t="s">
-        <v>716</v>
-      </c>
-      <c r="I95">
-        <v>26</v>
-      </c>
-      <c r="J95">
-        <v>13818</v>
-      </c>
-      <c r="K95" t="s">
-        <v>717</v>
-      </c>
-      <c r="L95">
-        <v>1371</v>
-      </c>
       <c r="M95">
-        <v>1142</v>
+        <v>86</v>
       </c>
       <c r="N95">
-        <v>229</v>
+        <v>12</v>
       </c>
       <c r="O95">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="P95">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Q95">
-        <v>1614</v>
+        <v>100</v>
       </c>
       <c r="R95" t="s">
-        <v>269</v>
+        <v>210</v>
       </c>
       <c r="S95">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="T95">
         <v>0</v>
@@ -9854,63 +9747,63 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>714</v>
+      </c>
+      <c r="B96" t="s">
+        <v>83</v>
+      </c>
+      <c r="C96" t="s">
+        <v>204</v>
+      </c>
+      <c r="D96" t="s">
+        <v>715</v>
+      </c>
+      <c r="E96" t="s">
+        <v>715</v>
+      </c>
+      <c r="F96" t="s">
+        <v>716</v>
+      </c>
+      <c r="G96" t="s">
+        <v>717</v>
+      </c>
+      <c r="H96" t="s">
         <v>718</v>
       </c>
-      <c r="B96" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="I96">
+        <v>9</v>
+      </c>
+      <c r="J96">
+        <v>41045</v>
+      </c>
+      <c r="K96" t="s">
         <v>719</v>
       </c>
-      <c r="D96" t="s">
-        <v>720</v>
-      </c>
-      <c r="E96" t="s">
-        <v>83</v>
-      </c>
-      <c r="F96" t="s">
-        <v>721</v>
-      </c>
-      <c r="G96" t="s">
-        <v>722</v>
-      </c>
-      <c r="H96" t="s">
-        <v>723</v>
-      </c>
-      <c r="I96">
-        <v>1</v>
-      </c>
-      <c r="J96">
-        <v>1003232</v>
-      </c>
-      <c r="K96" t="s">
-        <v>724</v>
-      </c>
       <c r="L96">
-        <v>544</v>
+        <v>100</v>
       </c>
       <c r="M96">
-        <v>540</v>
+        <v>100</v>
       </c>
       <c r="N96">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O96">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="P96">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="Q96">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="R96" t="s">
-        <v>725</v>
+        <v>210</v>
       </c>
       <c r="S96">
-        <v>95</v>
-      </c>
-      <c r="T96" s="3">
+        <v>100</v>
+      </c>
+      <c r="T96">
         <v>0</v>
       </c>
       <c r="U96">
@@ -9928,63 +9821,63 @@
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C97" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="D97" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="E97" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="F97" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
       <c r="G97" t="s">
-        <v>730</v>
+        <v>723</v>
       </c>
       <c r="H97" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="I97">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="J97">
-        <v>8496</v>
+        <v>695850</v>
       </c>
       <c r="K97" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
       <c r="L97">
-        <v>6524</v>
+        <v>99</v>
       </c>
       <c r="M97">
-        <v>4968</v>
+        <v>99</v>
       </c>
       <c r="N97">
-        <v>1556</v>
+        <v>0</v>
       </c>
       <c r="O97">
-        <v>318</v>
+        <v>0</v>
       </c>
       <c r="P97">
-        <v>638</v>
+        <v>1</v>
       </c>
       <c r="Q97">
-        <v>7480</v>
+        <v>100</v>
       </c>
       <c r="R97" t="s">
-        <v>137</v>
+        <v>210</v>
       </c>
       <c r="S97">
-        <v>91</v>
-      </c>
-      <c r="T97" s="3">
+        <v>99</v>
+      </c>
+      <c r="T97">
         <v>0</v>
       </c>
       <c r="U97">
@@ -9999,379 +9892,6 @@
       <c r="X97" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>733</v>
-      </c>
-      <c r="B98" t="s">
-        <v>83</v>
-      </c>
-      <c r="C98" t="s">
-        <v>734</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>735</v>
-      </c>
-      <c r="E98" t="s">
-        <v>736</v>
-      </c>
-      <c r="F98" t="s">
-        <v>737</v>
-      </c>
-      <c r="G98" t="s">
-        <v>738</v>
-      </c>
-      <c r="H98" t="s">
-        <v>739</v>
-      </c>
-      <c r="I98">
-        <v>1</v>
-      </c>
-      <c r="J98">
-        <v>2005467</v>
-      </c>
-      <c r="K98" t="s">
-        <v>740</v>
-      </c>
-      <c r="L98">
-        <v>1886</v>
-      </c>
-      <c r="M98">
-        <v>1879</v>
-      </c>
-      <c r="N98">
-        <v>7</v>
-      </c>
-      <c r="O98">
-        <v>2</v>
-      </c>
-      <c r="P98">
-        <v>11</v>
-      </c>
-      <c r="Q98">
-        <v>1899</v>
-      </c>
-      <c r="R98" t="s">
-        <v>741</v>
-      </c>
-      <c r="S98">
-        <v>99</v>
-      </c>
-      <c r="T98" s="3">
-        <v>50</v>
-      </c>
-      <c r="U98">
-        <v>0</v>
-      </c>
-      <c r="V98">
-        <v>0</v>
-      </c>
-      <c r="W98">
-        <v>0</v>
-      </c>
-      <c r="X98" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>203</v>
-      </c>
-      <c r="B99" t="s">
-        <v>83</v>
-      </c>
-      <c r="C99" t="s">
-        <v>204</v>
-      </c>
-      <c r="D99" t="s">
-        <v>205</v>
-      </c>
-      <c r="E99" t="s">
-        <v>205</v>
-      </c>
-      <c r="F99" t="s">
-        <v>206</v>
-      </c>
-      <c r="G99" t="s">
-        <v>207</v>
-      </c>
-      <c r="H99" t="s">
-        <v>208</v>
-      </c>
-      <c r="I99">
-        <v>14</v>
-      </c>
-      <c r="J99">
-        <v>403677</v>
-      </c>
-      <c r="K99" t="s">
-        <v>209</v>
-      </c>
-      <c r="L99">
-        <v>100</v>
-      </c>
-      <c r="M99">
-        <v>99</v>
-      </c>
-      <c r="N99">
-        <v>1</v>
-      </c>
-      <c r="O99">
-        <v>0</v>
-      </c>
-      <c r="P99">
-        <v>0</v>
-      </c>
-      <c r="Q99">
-        <v>100</v>
-      </c>
-      <c r="R99" t="s">
-        <v>210</v>
-      </c>
-      <c r="S99">
-        <v>100</v>
-      </c>
-      <c r="T99" s="3">
-        <v>46</v>
-      </c>
-      <c r="U99">
-        <v>0</v>
-      </c>
-      <c r="V99">
-        <v>0</v>
-      </c>
-      <c r="W99">
-        <v>0</v>
-      </c>
-      <c r="X99" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>742</v>
-      </c>
-      <c r="B100" t="s">
-        <v>83</v>
-      </c>
-      <c r="C100" t="s">
-        <v>204</v>
-      </c>
-      <c r="D100" t="s">
-        <v>743</v>
-      </c>
-      <c r="E100" t="s">
-        <v>743</v>
-      </c>
-      <c r="F100" t="s">
-        <v>744</v>
-      </c>
-      <c r="G100" t="s">
-        <v>745</v>
-      </c>
-      <c r="H100" t="s">
-        <v>746</v>
-      </c>
-      <c r="I100">
-        <v>4</v>
-      </c>
-      <c r="J100">
-        <v>65357</v>
-      </c>
-      <c r="K100" t="s">
-        <v>746</v>
-      </c>
-      <c r="L100">
-        <v>98</v>
-      </c>
-      <c r="M100">
-        <v>86</v>
-      </c>
-      <c r="N100">
-        <v>12</v>
-      </c>
-      <c r="O100">
-        <v>2</v>
-      </c>
-      <c r="P100">
-        <v>0</v>
-      </c>
-      <c r="Q100">
-        <v>100</v>
-      </c>
-      <c r="R100" t="s">
-        <v>210</v>
-      </c>
-      <c r="S100">
-        <v>100</v>
-      </c>
-      <c r="T100" s="3">
-        <v>0</v>
-      </c>
-      <c r="U100">
-        <v>0</v>
-      </c>
-      <c r="V100">
-        <v>0</v>
-      </c>
-      <c r="W100">
-        <v>0</v>
-      </c>
-      <c r="X100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>747</v>
-      </c>
-      <c r="B101" t="s">
-        <v>83</v>
-      </c>
-      <c r="C101" t="s">
-        <v>204</v>
-      </c>
-      <c r="D101" t="s">
-        <v>748</v>
-      </c>
-      <c r="E101" t="s">
-        <v>748</v>
-      </c>
-      <c r="F101" t="s">
-        <v>749</v>
-      </c>
-      <c r="G101" t="s">
-        <v>750</v>
-      </c>
-      <c r="H101" t="s">
-        <v>751</v>
-      </c>
-      <c r="I101">
-        <v>9</v>
-      </c>
-      <c r="J101">
-        <v>41045</v>
-      </c>
-      <c r="K101" t="s">
-        <v>752</v>
-      </c>
-      <c r="L101">
-        <v>100</v>
-      </c>
-      <c r="M101">
-        <v>100</v>
-      </c>
-      <c r="N101">
-        <v>0</v>
-      </c>
-      <c r="O101">
-        <v>0</v>
-      </c>
-      <c r="P101">
-        <v>0</v>
-      </c>
-      <c r="Q101">
-        <v>100</v>
-      </c>
-      <c r="R101" t="s">
-        <v>210</v>
-      </c>
-      <c r="S101">
-        <v>100</v>
-      </c>
-      <c r="T101" s="3">
-        <v>0</v>
-      </c>
-      <c r="U101">
-        <v>0</v>
-      </c>
-      <c r="V101">
-        <v>0</v>
-      </c>
-      <c r="W101">
-        <v>0</v>
-      </c>
-      <c r="X101" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>753</v>
-      </c>
-      <c r="B102" t="s">
-        <v>83</v>
-      </c>
-      <c r="C102" t="s">
-        <v>204</v>
-      </c>
-      <c r="D102" t="s">
-        <v>754</v>
-      </c>
-      <c r="E102" t="s">
-        <v>754</v>
-      </c>
-      <c r="F102" t="s">
-        <v>755</v>
-      </c>
-      <c r="G102" t="s">
-        <v>756</v>
-      </c>
-      <c r="H102" t="s">
-        <v>757</v>
-      </c>
-      <c r="I102">
-        <v>18</v>
-      </c>
-      <c r="J102">
-        <v>695850</v>
-      </c>
-      <c r="K102" t="s">
-        <v>758</v>
-      </c>
-      <c r="L102">
-        <v>99</v>
-      </c>
-      <c r="M102">
-        <v>99</v>
-      </c>
-      <c r="N102">
-        <v>0</v>
-      </c>
-      <c r="O102">
-        <v>0</v>
-      </c>
-      <c r="P102">
-        <v>1</v>
-      </c>
-      <c r="Q102">
-        <v>100</v>
-      </c>
-      <c r="R102" t="s">
-        <v>210</v>
-      </c>
-      <c r="S102">
-        <v>99</v>
-      </c>
-      <c r="T102" s="3">
-        <v>0</v>
-      </c>
-      <c r="U102">
-        <v>0</v>
-      </c>
-      <c r="V102">
-        <v>0</v>
-      </c>
-      <c r="W102">
-        <v>0</v>
-      </c>
-      <c r="X102" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="T103" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1">
@@ -12322,78 +11842,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D82">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="45">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D2479778-92BD-5646-BA3C-964A2E05C21E}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D83">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="43">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BA52B593-2146-E144-8AA3-702975CE0067}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D84">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="41">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1FE5A174-6E60-DC4A-94DC-EE28EC789F85}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -12417,7 +11865,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D86">
+  <conditionalFormatting sqref="D83">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -12441,7 +11889,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D87">
+  <conditionalFormatting sqref="D84">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -12465,7 +11913,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D88">
+  <conditionalFormatting sqref="D85">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -12489,31 +11937,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D89">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="33">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{51BEEA3A-63A4-5645-8991-655182006041}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D90">
+  <conditionalFormatting sqref="D86">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -12537,7 +11961,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D91">
+  <conditionalFormatting sqref="D87">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -12561,7 +11985,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D92">
+  <conditionalFormatting sqref="D88">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -12585,7 +12009,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D93">
+  <conditionalFormatting sqref="D89">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -12609,7 +12033,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D94">
+  <conditionalFormatting sqref="D90">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -12633,8 +12057,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D95">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="S1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12644,21 +12068,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="23">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B3E8C792-A0CB-B74E-B096-D5F250E89A83}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="S1:S1048576">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12669,8 +12081,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="T91:T97 S87:S90 S63:S82 S40:S53 S84:S85 S36:S37 S55:S61 S2:S3 S14:S34 S9:S12 S6">
+    <cfRule type="colorScale" priority="205">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12681,22 +12093,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S91:S95 T96:T102 S63:S85 S40:S53 S87:S89 S36:S37 S55:S61 S2:S3 S14:S34 S9:S12 S6">
-    <cfRule type="colorScale" priority="205">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D98" r:id="rId1" display="https://en.wikipedia.org/wiki/Cyanobacteria" xr:uid="{19BA12DF-A3BB-8D4B-96A4-4ACCB92037F1}"/>
+    <hyperlink ref="D93" r:id="rId1" display="https://en.wikipedia.org/wiki/Cyanobacteria" xr:uid="{19BA12DF-A3BB-8D4B-96A4-4ACCB92037F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -13754,7 +13155,7 @@
           <xm:sqref>D81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D2479778-92BD-5646-BA3C-964A2E05C21E}">
+          <x14:cfRule type="dataBar" id="{DAFBB8AB-FABD-B34D-A54B-5811FA139F3E}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13767,7 +13168,7 @@
           <xm:sqref>D82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BA52B593-2146-E144-8AA3-702975CE0067}">
+          <x14:cfRule type="dataBar" id="{0C11BB59-368E-874B-B7E3-AD315ABEA4C3}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13780,7 +13181,7 @@
           <xm:sqref>D83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1FE5A174-6E60-DC4A-94DC-EE28EC789F85}">
+          <x14:cfRule type="dataBar" id="{F959970D-9B0A-2946-94A4-50451AACAFF5}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13793,7 +13194,7 @@
           <xm:sqref>D84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DAFBB8AB-FABD-B34D-A54B-5811FA139F3E}">
+          <x14:cfRule type="dataBar" id="{FD9E73EB-9C57-2D4F-8A20-72A9D2C0B114}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13806,7 +13207,7 @@
           <xm:sqref>D85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0C11BB59-368E-874B-B7E3-AD315ABEA4C3}">
+          <x14:cfRule type="dataBar" id="{46E32D18-4F0F-CF44-A5DA-41764EF960D8}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13819,7 +13220,7 @@
           <xm:sqref>D86</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F959970D-9B0A-2946-94A4-50451AACAFF5}">
+          <x14:cfRule type="dataBar" id="{31AB5E9D-8184-2E46-816F-019C22A426AE}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13832,7 +13233,7 @@
           <xm:sqref>D87</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FD9E73EB-9C57-2D4F-8A20-72A9D2C0B114}">
+          <x14:cfRule type="dataBar" id="{60CCE12D-4661-1940-8F94-C9EF08188B71}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13845,7 +13246,7 @@
           <xm:sqref>D88</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{51BEEA3A-63A4-5645-8991-655182006041}">
+          <x14:cfRule type="dataBar" id="{2281BEAE-AB1D-F74F-8792-EBC84EFC8177}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13858,7 +13259,7 @@
           <xm:sqref>D89</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{46E32D18-4F0F-CF44-A5DA-41764EF960D8}">
+          <x14:cfRule type="dataBar" id="{7AA82AF5-A405-124B-ABF5-E29428FDAFE4}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13870,71 +13271,6 @@
           </x14:cfRule>
           <xm:sqref>D90</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{31AB5E9D-8184-2E46-816F-019C22A426AE}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D91</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{60CCE12D-4661-1940-8F94-C9EF08188B71}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D92</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2281BEAE-AB1D-F74F-8792-EBC84EFC8177}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D93</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7AA82AF5-A405-124B-ABF5-E29428FDAFE4}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D94</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B3E8C792-A0CB-B74E-B096-D5F250E89A83}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D95</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
new proteome tree data
</commit_message>
<xml_diff>
--- a/data/proteome-tree/class-representatives.xlsx
+++ b/data/proteome-tree/class-representatives.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idamei/polyphenol-oxidases/data/proteome-tree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D820B613-F968-BC4F-9704-57A81D9C8915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A14715-3D88-6F47-B8C1-B962A728C378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{F5F2D1A1-B58F-E84D-BA53-6173843C03DE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="38400" windowHeight="18880" xr2:uid="{F5F2D1A1-B58F-E84D-BA53-6173843C03DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="754">
   <si>
     <t>UP000077248</t>
   </si>
@@ -2295,6 +2295,9 @@
   </si>
   <si>
     <t>Glutinoglossum americanum</t>
+  </si>
+  <si>
+    <t>completeness_score</t>
   </si>
 </sst>
 </file>
@@ -2363,7 +2366,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2704,10 +2717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55AD071-326A-564C-9452-BA0C45FD02D7}">
-  <dimension ref="A1:X97"/>
+  <dimension ref="A1:Y97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="H57" workbookViewId="0">
+      <selection activeCell="U81" sqref="U81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2715,7 +2728,7 @@
     <col min="8" max="8" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>726</v>
       </c>
@@ -2788,8 +2801,11 @@
       <c r="X1" t="s">
         <v>749</v>
       </c>
+      <c r="Y1" t="s">
+        <v>753</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2862,8 +2878,12 @@
       <c r="X2" t="s">
         <v>10</v>
       </c>
+      <c r="Y2" s="1">
+        <f>L2*100/Q2</f>
+        <v>98.689956331877724</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2936,8 +2956,12 @@
       <c r="X3" t="s">
         <v>19</v>
       </c>
+      <c r="Y3" s="1">
+        <f t="shared" ref="Y3:Y66" si="0">L3*100/Q3</f>
+        <v>95.538057742782158</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>750</v>
       </c>
@@ -3010,8 +3034,12 @@
       <c r="X4" t="s">
         <v>24</v>
       </c>
+      <c r="Y4" s="1">
+        <f t="shared" si="0"/>
+        <v>88.921453692848772</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3084,8 +3112,12 @@
       <c r="X5" t="s">
         <v>24</v>
       </c>
+      <c r="Y5" s="1">
+        <f t="shared" si="0"/>
+        <v>95.603751465416181</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3158,8 +3190,12 @@
       <c r="X6" t="s">
         <v>24</v>
       </c>
+      <c r="Y6" s="1">
+        <f t="shared" si="0"/>
+        <v>99.787521730732081</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -3232,8 +3268,12 @@
       <c r="X7" t="s">
         <v>24</v>
       </c>
+      <c r="Y7" s="1">
+        <f t="shared" si="0"/>
+        <v>96.072684642438446</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -3306,8 +3346,12 @@
       <c r="X8" t="s">
         <v>24</v>
       </c>
+      <c r="Y8" s="1">
+        <f t="shared" si="0"/>
+        <v>95.486518171160611</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -3380,8 +3424,12 @@
       <c r="X9" t="s">
         <v>61</v>
       </c>
+      <c r="Y9" s="1">
+        <f t="shared" si="0"/>
+        <v>98.46461949265688</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -3454,8 +3502,12 @@
       <c r="X10" t="s">
         <v>24</v>
       </c>
+      <c r="Y10" s="1">
+        <f t="shared" si="0"/>
+        <v>94.108527131782949</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -3528,8 +3580,12 @@
       <c r="X11" t="s">
         <v>24</v>
       </c>
+      <c r="Y11" s="1">
+        <f t="shared" si="0"/>
+        <v>99.43310657596372</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -3602,8 +3658,12 @@
       <c r="X12" t="s">
         <v>24</v>
       </c>
+      <c r="Y12" s="1">
+        <f t="shared" si="0"/>
+        <v>89.709762532981529</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -3676,8 +3736,12 @@
       <c r="X13" t="s">
         <v>24</v>
       </c>
+      <c r="Y13" s="1">
+        <f t="shared" si="0"/>
+        <v>94.609665427509299</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -3750,8 +3814,12 @@
       <c r="X14" t="s">
         <v>24</v>
       </c>
+      <c r="Y14" s="1">
+        <f t="shared" si="0"/>
+        <v>97.747252747252745</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -3824,8 +3892,12 @@
       <c r="X15" t="s">
         <v>24</v>
       </c>
+      <c r="Y15" s="1">
+        <f t="shared" si="0"/>
+        <v>97.702448210922782</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -3898,8 +3970,12 @@
       <c r="X16" t="s">
         <v>24</v>
       </c>
+      <c r="Y16" s="1">
+        <f t="shared" si="0"/>
+        <v>98.260973854641406</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3972,8 +4048,12 @@
       <c r="X17" t="s">
         <v>24</v>
       </c>
+      <c r="Y17" s="1">
+        <f t="shared" si="0"/>
+        <v>90.041741204531903</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4046,8 +4126,12 @@
       <c r="X18" t="s">
         <v>24</v>
       </c>
+      <c r="Y18" s="1">
+        <f t="shared" si="0"/>
+        <v>86.310160427807489</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -4120,8 +4204,12 @@
       <c r="X19" t="s">
         <v>24</v>
       </c>
+      <c r="Y19" s="1">
+        <f t="shared" si="0"/>
+        <v>99.484760522496373</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -4194,8 +4282,12 @@
       <c r="X20" t="s">
         <v>24</v>
       </c>
+      <c r="Y20" s="1">
+        <f t="shared" si="0"/>
+        <v>98.742138364779876</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -4268,8 +4360,12 @@
       <c r="X21" t="s">
         <v>24</v>
       </c>
+      <c r="Y21" s="1">
+        <f t="shared" si="0"/>
+        <v>80.132200188857411</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>164</v>
       </c>
@@ -4342,8 +4438,12 @@
       <c r="X22" t="s">
         <v>24</v>
       </c>
+      <c r="Y22" s="1">
+        <f t="shared" si="0"/>
+        <v>90.840415486307833</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>171</v>
       </c>
@@ -4416,8 +4516,12 @@
       <c r="X23" t="s">
         <v>24</v>
       </c>
+      <c r="Y23" s="1">
+        <f t="shared" si="0"/>
+        <v>88.366383380547688</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>177</v>
       </c>
@@ -4490,8 +4594,12 @@
       <c r="X24" t="s">
         <v>24</v>
       </c>
+      <c r="Y24" s="1">
+        <f t="shared" si="0"/>
+        <v>99.968061322261264</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -4564,8 +4672,12 @@
       <c r="X25" t="s">
         <v>194</v>
       </c>
+      <c r="Y25" s="1">
+        <f t="shared" si="0"/>
+        <v>99.303356554781502</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>195</v>
       </c>
@@ -4638,8 +4750,12 @@
       <c r="X26" t="s">
         <v>19</v>
       </c>
+      <c r="Y26" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>211</v>
       </c>
@@ -4712,8 +4828,12 @@
       <c r="X27" t="s">
         <v>220</v>
       </c>
+      <c r="Y27" s="1">
+        <f t="shared" si="0"/>
+        <v>98.709344346928233</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>221</v>
       </c>
@@ -4786,8 +4906,12 @@
       <c r="X28" t="s">
         <v>220</v>
       </c>
+      <c r="Y28" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>229</v>
       </c>
@@ -4860,8 +4984,12 @@
       <c r="X29" t="s">
         <v>24</v>
       </c>
+      <c r="Y29" s="1">
+        <f t="shared" si="0"/>
+        <v>99.613899613899619</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>236</v>
       </c>
@@ -4934,8 +5062,12 @@
       <c r="X30" t="s">
         <v>220</v>
       </c>
+      <c r="Y30" s="1">
+        <f t="shared" si="0"/>
+        <v>99.488491048593346</v>
+      </c>
     </row>
-    <row r="31" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>243</v>
       </c>
@@ -5008,8 +5140,12 @@
       <c r="X31" t="s">
         <v>24</v>
       </c>
+      <c r="Y31" s="1">
+        <f t="shared" si="0"/>
+        <v>93.725490196078425</v>
+      </c>
     </row>
-    <row r="32" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>252</v>
       </c>
@@ -5082,8 +5218,12 @@
       <c r="X32" t="s">
         <v>24</v>
       </c>
+      <c r="Y32" s="1">
+        <f t="shared" si="0"/>
+        <v>98.925193465176264</v>
+      </c>
     </row>
-    <row r="33" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>262</v>
       </c>
@@ -5156,8 +5296,12 @@
       <c r="X33" t="s">
         <v>24</v>
       </c>
+      <c r="Y33" s="1">
+        <f t="shared" si="0"/>
+        <v>88.723667905824044</v>
+      </c>
     </row>
-    <row r="34" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>270</v>
       </c>
@@ -5230,8 +5374,12 @@
       <c r="X34" t="s">
         <v>24</v>
       </c>
+      <c r="Y34" s="1">
+        <f t="shared" si="0"/>
+        <v>98.946675444371294</v>
+      </c>
     </row>
-    <row r="35" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>279</v>
       </c>
@@ -5304,8 +5452,12 @@
       <c r="X35" t="s">
         <v>24</v>
       </c>
+      <c r="Y35" s="1">
+        <f t="shared" si="0"/>
+        <v>96.541950113378689</v>
+      </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>286</v>
       </c>
@@ -5378,8 +5530,12 @@
       <c r="X36" t="s">
         <v>24</v>
       </c>
+      <c r="Y36" s="1">
+        <f t="shared" si="0"/>
+        <v>95.804988662131521</v>
+      </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>292</v>
       </c>
@@ -5452,8 +5608,12 @@
       <c r="X37" t="s">
         <v>24</v>
       </c>
+      <c r="Y37" s="1">
+        <f t="shared" si="0"/>
+        <v>94.897959183673464</v>
+      </c>
     </row>
-    <row r="38" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>299</v>
       </c>
@@ -5526,8 +5686,12 @@
       <c r="X38" t="s">
         <v>220</v>
       </c>
+      <c r="Y38" s="1">
+        <f t="shared" si="0"/>
+        <v>80.612244897959187</v>
+      </c>
     </row>
-    <row r="39" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>305</v>
       </c>
@@ -5600,8 +5764,12 @@
       <c r="X39" t="s">
         <v>24</v>
       </c>
+      <c r="Y39" s="1">
+        <f t="shared" si="0"/>
+        <v>93.494423791821561</v>
+      </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>311</v>
       </c>
@@ -5674,8 +5842,12 @@
       <c r="X40" t="s">
         <v>24</v>
       </c>
+      <c r="Y40" s="1">
+        <f t="shared" si="0"/>
+        <v>97.361477572559366</v>
+      </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>319</v>
       </c>
@@ -5748,8 +5920,12 @@
       <c r="X41" t="s">
         <v>24</v>
       </c>
+      <c r="Y41" s="1">
+        <f t="shared" si="0"/>
+        <v>80.079155672823219</v>
+      </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>325</v>
       </c>
@@ -5822,8 +5998,12 @@
       <c r="X42" t="s">
         <v>24</v>
       </c>
+      <c r="Y42" s="1">
+        <f t="shared" si="0"/>
+        <v>79.815303430079155</v>
+      </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>332</v>
       </c>
@@ -5896,8 +6076,12 @@
       <c r="X43" t="s">
         <v>61</v>
       </c>
+      <c r="Y43" s="1">
+        <f t="shared" si="0"/>
+        <v>87.203166226912927</v>
+      </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>339</v>
       </c>
@@ -5970,8 +6154,12 @@
       <c r="X44" t="s">
         <v>24</v>
       </c>
+      <c r="Y44" s="1">
+        <f t="shared" si="0"/>
+        <v>73.218997361477577</v>
+      </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>345</v>
       </c>
@@ -6044,8 +6232,12 @@
       <c r="X45" t="s">
         <v>24</v>
       </c>
+      <c r="Y45" s="1">
+        <f t="shared" si="0"/>
+        <v>90.25157232704403</v>
+      </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>353</v>
       </c>
@@ -6118,8 +6310,12 @@
       <c r="X46" t="s">
         <v>24</v>
       </c>
+      <c r="Y46" s="1">
+        <f t="shared" si="0"/>
+        <v>94.968553459119491</v>
+      </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>359</v>
       </c>
@@ -6192,8 +6388,12 @@
       <c r="X47" t="s">
         <v>24</v>
       </c>
+      <c r="Y47" s="1">
+        <f t="shared" si="0"/>
+        <v>96.012269938650306</v>
+      </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>368</v>
       </c>
@@ -6266,8 +6466,12 @@
       <c r="X48" t="s">
         <v>24</v>
       </c>
+      <c r="Y48" s="1">
+        <f t="shared" si="0"/>
+        <v>79.151426481346007</v>
+      </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>376</v>
       </c>
@@ -6340,8 +6544,12 @@
       <c r="X49" t="s">
         <v>24</v>
       </c>
+      <c r="Y49" s="1">
+        <f t="shared" si="0"/>
+        <v>98.63731656184487</v>
+      </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>384</v>
       </c>
@@ -6414,8 +6622,12 @@
       <c r="X50" t="s">
         <v>24</v>
       </c>
+      <c r="Y50" s="1">
+        <f t="shared" si="0"/>
+        <v>76.205450733752627</v>
+      </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>392</v>
       </c>
@@ -6488,8 +6700,12 @@
       <c r="X51" t="s">
         <v>24</v>
       </c>
+      <c r="Y51" s="1">
+        <f t="shared" si="0"/>
+        <v>78.721174004192875</v>
+      </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>399</v>
       </c>
@@ -6562,8 +6778,12 @@
       <c r="X52" t="s">
         <v>24</v>
       </c>
+      <c r="Y52" s="1">
+        <f t="shared" si="0"/>
+        <v>90.686813186813183</v>
+      </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>406</v>
       </c>
@@ -6636,8 +6856,12 @@
       <c r="X53" t="s">
         <v>24</v>
       </c>
+      <c r="Y53" s="1">
+        <f t="shared" si="0"/>
+        <v>97.484276729559753</v>
+      </c>
     </row>
-    <row r="54" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>413</v>
       </c>
@@ -6710,8 +6934,12 @@
       <c r="X54" t="s">
         <v>24</v>
       </c>
+      <c r="Y54" s="1">
+        <f t="shared" si="0"/>
+        <v>87.735849056603769</v>
+      </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>421</v>
       </c>
@@ -6784,8 +7012,12 @@
       <c r="X55" t="s">
         <v>24</v>
       </c>
+      <c r="Y55" s="1">
+        <f t="shared" si="0"/>
+        <v>81.132075471698116</v>
+      </c>
     </row>
-    <row r="56" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>427</v>
       </c>
@@ -6858,8 +7090,12 @@
       <c r="X56" t="s">
         <v>24</v>
       </c>
+      <c r="Y56" s="1">
+        <f t="shared" si="0"/>
+        <v>99.371069182389931</v>
+      </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>434</v>
       </c>
@@ -6932,8 +7168,12 @@
       <c r="X57" t="s">
         <v>24</v>
       </c>
+      <c r="Y57" s="1">
+        <f t="shared" si="0"/>
+        <v>91.299790356394126</v>
+      </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>441</v>
       </c>
@@ -7006,8 +7246,12 @@
       <c r="X58" t="s">
         <v>24</v>
       </c>
+      <c r="Y58" s="1">
+        <f t="shared" si="0"/>
+        <v>89.832285115303989</v>
+      </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>449</v>
       </c>
@@ -7080,8 +7324,12 @@
       <c r="X59" t="s">
         <v>24</v>
       </c>
+      <c r="Y59" s="1">
+        <f t="shared" si="0"/>
+        <v>82.809224318658281</v>
+      </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>456</v>
       </c>
@@ -7154,8 +7402,12 @@
       <c r="X60" t="s">
         <v>61</v>
       </c>
+      <c r="Y60" s="1">
+        <f t="shared" si="0"/>
+        <v>99.168053244592343</v>
+      </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>464</v>
       </c>
@@ -7228,8 +7480,12 @@
       <c r="X61" t="s">
         <v>24</v>
       </c>
+      <c r="Y61" s="1">
+        <f t="shared" si="0"/>
+        <v>87.354409317803658</v>
+      </c>
     </row>
-    <row r="62" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>470</v>
       </c>
@@ -7302,8 +7558,12 @@
       <c r="X62" t="s">
         <v>24</v>
       </c>
+      <c r="Y62" s="1">
+        <f t="shared" si="0"/>
+        <v>96.774193548387103</v>
+      </c>
     </row>
-    <row r="63" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>478</v>
       </c>
@@ -7376,8 +7636,12 @@
       <c r="X63" t="s">
         <v>24</v>
       </c>
+      <c r="Y63" s="1">
+        <f t="shared" si="0"/>
+        <v>86.290322580645167</v>
+      </c>
     </row>
-    <row r="64" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>486</v>
       </c>
@@ -7450,8 +7714,12 @@
       <c r="X64" t="s">
         <v>24</v>
       </c>
+      <c r="Y64" s="1">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
     </row>
-    <row r="65" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>494</v>
       </c>
@@ -7524,8 +7792,12 @@
       <c r="X65" t="s">
         <v>24</v>
       </c>
+      <c r="Y65" s="1">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
     </row>
-    <row r="66" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>501</v>
       </c>
@@ -7598,8 +7870,12 @@
       <c r="X66" t="s">
         <v>220</v>
       </c>
+      <c r="Y66" s="1">
+        <f t="shared" si="0"/>
+        <v>98.756218905472636</v>
+      </c>
     </row>
-    <row r="67" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>509</v>
       </c>
@@ -7672,8 +7948,12 @@
       <c r="X67" t="s">
         <v>19</v>
       </c>
+      <c r="Y67" s="1">
+        <f t="shared" ref="Y67:Y97" si="1">L67*100/Q67</f>
+        <v>99.088541666666671</v>
+      </c>
     </row>
-    <row r="68" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>516</v>
       </c>
@@ -7746,8 +8026,12 @@
       <c r="X68" t="s">
         <v>24</v>
       </c>
+      <c r="Y68" s="1">
+        <f t="shared" si="1"/>
+        <v>96.268656716417908</v>
+      </c>
     </row>
-    <row r="69" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>523</v>
       </c>
@@ -7820,8 +8104,12 @@
       <c r="X69" t="s">
         <v>19</v>
       </c>
+      <c r="Y69" s="1">
+        <f t="shared" si="1"/>
+        <v>96.722846441947567</v>
+      </c>
     </row>
-    <row r="70" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>530</v>
       </c>
@@ -7894,8 +8182,12 @@
       <c r="X70" t="s">
         <v>24</v>
       </c>
+      <c r="Y70" s="1">
+        <f t="shared" si="1"/>
+        <v>94.833948339483399</v>
+      </c>
     </row>
-    <row r="71" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>538</v>
       </c>
@@ -7968,8 +8260,12 @@
       <c r="X71" t="s">
         <v>24</v>
       </c>
+      <c r="Y71" s="1">
+        <f t="shared" si="1"/>
+        <v>92.397660818713447</v>
+      </c>
     </row>
-    <row r="72" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>547</v>
       </c>
@@ -8042,8 +8338,12 @@
       <c r="X72" t="s">
         <v>24</v>
       </c>
+      <c r="Y72" s="1">
+        <f t="shared" si="1"/>
+        <v>97.076023391812868</v>
+      </c>
     </row>
-    <row r="73" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>554</v>
       </c>
@@ -8116,8 +8416,12 @@
       <c r="X73" t="s">
         <v>61</v>
       </c>
+      <c r="Y73" s="1">
+        <f t="shared" si="1"/>
+        <v>87.903225806451616</v>
+      </c>
     </row>
-    <row r="74" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>562</v>
       </c>
@@ -8190,8 +8494,12 @@
       <c r="X74" t="s">
         <v>24</v>
       </c>
+      <c r="Y74" s="1">
+        <f t="shared" si="1"/>
+        <v>89.019607843137251</v>
+      </c>
     </row>
-    <row r="75" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>570</v>
       </c>
@@ -8264,8 +8572,12 @@
       <c r="X75" t="s">
         <v>220</v>
       </c>
+      <c r="Y75" s="1">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="76" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>579</v>
       </c>
@@ -8338,8 +8650,12 @@
       <c r="X76" t="s">
         <v>24</v>
       </c>
+      <c r="Y76" s="1">
+        <f t="shared" si="1"/>
+        <v>96.969696969696969</v>
+      </c>
     </row>
-    <row r="77" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>586</v>
       </c>
@@ -8412,8 +8728,12 @@
       <c r="X77" t="s">
         <v>24</v>
       </c>
+      <c r="Y77" s="1">
+        <f t="shared" si="1"/>
+        <v>91.935483870967744</v>
+      </c>
     </row>
-    <row r="78" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>593</v>
       </c>
@@ -8486,8 +8806,12 @@
       <c r="X78" t="s">
         <v>24</v>
       </c>
+      <c r="Y78" s="1">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
     </row>
-    <row r="79" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>599</v>
       </c>
@@ -8560,8 +8884,12 @@
       <c r="X79" t="s">
         <v>24</v>
       </c>
+      <c r="Y79" s="1">
+        <f t="shared" si="1"/>
+        <v>83.137254901960787</v>
+      </c>
     </row>
-    <row r="80" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>606</v>
       </c>
@@ -8634,8 +8962,12 @@
       <c r="X80" t="s">
         <v>24</v>
       </c>
+      <c r="Y80" s="1">
+        <f t="shared" si="1"/>
+        <v>70.175438596491233</v>
+      </c>
     </row>
-    <row r="81" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>613</v>
       </c>
@@ -8708,8 +9040,12 @@
       <c r="X81" t="s">
         <v>24</v>
       </c>
+      <c r="Y81" s="1">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
     </row>
-    <row r="82" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>619</v>
       </c>
@@ -8782,8 +9118,12 @@
       <c r="X82" t="s">
         <v>24</v>
       </c>
+      <c r="Y82" s="1">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
     </row>
-    <row r="83" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>625</v>
       </c>
@@ -8856,8 +9196,12 @@
       <c r="X83" t="s">
         <v>24</v>
       </c>
+      <c r="Y83" s="1">
+        <f t="shared" si="1"/>
+        <v>99.474605954465844</v>
+      </c>
     </row>
-    <row r="84" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>634</v>
       </c>
@@ -8930,8 +9274,12 @@
       <c r="X84" t="s">
         <v>24</v>
       </c>
+      <c r="Y84" s="1">
+        <f t="shared" si="1"/>
+        <v>78.039215686274517</v>
+      </c>
     </row>
-    <row r="85" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>642</v>
       </c>
@@ -9004,8 +9352,12 @@
       <c r="X85" t="s">
         <v>24</v>
       </c>
+      <c r="Y85" s="1">
+        <f t="shared" si="1"/>
+        <v>80.784313725490193</v>
+      </c>
     </row>
-    <row r="86" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>648</v>
       </c>
@@ -9078,8 +9430,12 @@
       <c r="X86" t="s">
         <v>61</v>
       </c>
+      <c r="Y86" s="1">
+        <f t="shared" si="1"/>
+        <v>97.87685774946921</v>
+      </c>
     </row>
-    <row r="87" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>656</v>
       </c>
@@ -9152,8 +9508,12 @@
       <c r="X87" t="s">
         <v>24</v>
       </c>
+      <c r="Y87" s="1">
+        <f t="shared" si="1"/>
+        <v>92.890059249506251</v>
+      </c>
     </row>
-    <row r="88" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>663</v>
       </c>
@@ -9226,8 +9586,12 @@
       <c r="X88" t="s">
         <v>24</v>
       </c>
+      <c r="Y88" s="1">
+        <f t="shared" si="1"/>
+        <v>72.235294117647058</v>
+      </c>
     </row>
-    <row r="89" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>671</v>
       </c>
@@ -9300,8 +9664,12 @@
       <c r="X89" t="s">
         <v>24</v>
       </c>
+      <c r="Y89" s="1">
+        <f t="shared" si="1"/>
+        <v>96.941176470588232</v>
+      </c>
     </row>
-    <row r="90" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>678</v>
       </c>
@@ -9374,8 +9742,12 @@
       <c r="X90" t="s">
         <v>24</v>
       </c>
+      <c r="Y90" s="1">
+        <f t="shared" si="1"/>
+        <v>79.925650557620813</v>
+      </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>685</v>
       </c>
@@ -9448,8 +9820,12 @@
       <c r="X91" t="s">
         <v>24</v>
       </c>
+      <c r="Y91" s="1">
+        <f t="shared" si="1"/>
+        <v>90.666666666666671</v>
+      </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>693</v>
       </c>
@@ -9522,8 +9898,12 @@
       <c r="X92" t="s">
         <v>24</v>
       </c>
+      <c r="Y92" s="1">
+        <f t="shared" si="1"/>
+        <v>87.219251336898395</v>
+      </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>700</v>
       </c>
@@ -9596,8 +9976,12 @@
       <c r="X93" t="s">
         <v>61</v>
       </c>
+      <c r="Y93" s="1">
+        <f t="shared" si="1"/>
+        <v>99.315429173249072</v>
+      </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>203</v>
       </c>
@@ -9670,8 +10054,12 @@
       <c r="X94" t="s">
         <v>19</v>
       </c>
+      <c r="Y94" s="1">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>709</v>
       </c>
@@ -9744,8 +10132,12 @@
       <c r="X95" t="s">
         <v>24</v>
       </c>
+      <c r="Y95" s="1">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>714</v>
       </c>
@@ -9818,8 +10210,12 @@
       <c r="X96" t="s">
         <v>24</v>
       </c>
+      <c r="Y96" s="1">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>720</v>
       </c>
@@ -9891,11 +10287,15 @@
       </c>
       <c r="X97" t="s">
         <v>24</v>
+      </c>
+      <c r="Y97" s="1">
+        <f t="shared" si="1"/>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9905,7 +10305,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9919,17 +10319,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="colorScale" priority="199">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="200">
+    <cfRule type="dataBar" priority="201">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9941,12 +10331,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3 D5:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="colorScale" priority="197">
+    <cfRule type="colorScale" priority="200">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9956,7 +10341,22 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="198">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3 D5:D1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="colorScale" priority="198">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="199">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9970,17 +10370,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9992,9 +10382,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="colorScale" priority="190">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10004,7 +10392,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="191">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="colorScale" priority="191">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="192">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10018,17 +10418,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="colorScale" priority="192">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="193">
+    <cfRule type="dataBar" priority="194">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10040,9 +10430,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="colorScale" priority="188">
+    <cfRule type="colorScale" priority="193">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10052,7 +10440,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="189">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="dataBar" priority="190">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10064,9 +10454,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="186">
+    <cfRule type="colorScale" priority="189">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10076,7 +10464,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="187">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="dataBar" priority="188">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10088,9 +10478,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="colorScale" priority="184">
+    <cfRule type="colorScale" priority="187">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10100,7 +10488,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="185">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="dataBar" priority="186">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10112,9 +10502,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="colorScale" priority="182">
+    <cfRule type="colorScale" priority="185">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10124,7 +10512,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="183">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="dataBar" priority="184">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10136,9 +10526,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="colorScale" priority="180">
+    <cfRule type="colorScale" priority="183">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10148,7 +10536,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="181">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="colorScale" priority="181">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="182">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10162,7 +10562,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="colorScale" priority="178">
+    <cfRule type="colorScale" priority="179">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10172,7 +10572,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="179">
+    <cfRule type="dataBar" priority="180">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10186,7 +10586,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="colorScale" priority="174">
+    <cfRule type="colorScale" priority="175">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10196,7 +10596,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="175">
+    <cfRule type="dataBar" priority="176">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10210,17 +10610,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="colorScale" priority="176">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="177">
+    <cfRule type="dataBar" priority="178">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10232,9 +10622,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="colorScale" priority="172">
+    <cfRule type="colorScale" priority="177">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10244,7 +10632,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="173">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="colorScale" priority="173">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="174">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10258,17 +10658,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="colorScale" priority="170">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="171">
+    <cfRule type="dataBar" priority="172">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10280,9 +10670,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="colorScale" priority="168">
+    <cfRule type="colorScale" priority="171">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10292,7 +10680,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="169">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="dataBar" priority="170">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10304,9 +10694,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="colorScale" priority="166">
+    <cfRule type="colorScale" priority="169">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10316,7 +10704,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="167">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="colorScale" priority="167">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="168">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10330,7 +10730,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="colorScale" priority="164">
+    <cfRule type="colorScale" priority="165">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10340,7 +10740,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="165">
+    <cfRule type="dataBar" priority="166">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10354,17 +10754,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="colorScale" priority="162">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="163">
+    <cfRule type="dataBar" priority="164">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10376,9 +10766,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="colorScale" priority="160">
+    <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10388,7 +10776,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="161">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="dataBar" priority="162">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10400,9 +10790,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="colorScale" priority="158">
+    <cfRule type="colorScale" priority="161">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10412,7 +10800,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="159">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="colorScale" priority="159">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="160">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10426,17 +10826,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="colorScale" priority="156">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="157">
+    <cfRule type="dataBar" priority="158">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10448,9 +10838,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="colorScale" priority="154">
+    <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10460,7 +10848,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="155">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="dataBar" priority="156">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10472,9 +10862,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="colorScale" priority="150">
+    <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10484,7 +10872,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="151">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="dataBar" priority="152">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10496,9 +10886,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="colorScale" priority="148">
+    <cfRule type="colorScale" priority="151">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10508,7 +10896,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="149">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="dataBar" priority="150">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10520,9 +10910,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="colorScale" priority="144">
+    <cfRule type="colorScale" priority="149">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10532,7 +10920,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="145">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="dataBar" priority="146">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10544,9 +10934,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="colorScale" priority="142">
+    <cfRule type="colorScale" priority="145">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10556,7 +10944,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="143">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="dataBar" priority="144">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10568,9 +10958,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="colorScale" priority="140">
+    <cfRule type="colorScale" priority="143">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10580,7 +10968,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="141">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="colorScale" priority="141">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="142">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10594,7 +10994,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="colorScale" priority="138">
+    <cfRule type="colorScale" priority="139">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10604,7 +11004,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="139">
+    <cfRule type="dataBar" priority="140">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10618,17 +11018,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="colorScale" priority="136">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="137">
+    <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10640,9 +11030,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="colorScale" priority="130">
+    <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10652,7 +11040,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="131">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="dataBar" priority="132">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10664,9 +11054,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="colorScale" priority="132">
+    <cfRule type="colorScale" priority="131">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10676,7 +11064,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="133">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="dataBar" priority="134">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10688,9 +11078,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="colorScale" priority="134">
+    <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10700,7 +11088,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="135">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="136">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10712,9 +11102,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="135">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10724,7 +11112,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="11">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10736,9 +11126,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="colorScale" priority="128">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10748,7 +11136,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="129">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="dataBar" priority="130">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10760,9 +11150,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="colorScale" priority="126">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10772,7 +11160,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="127">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="dataBar" priority="128">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10784,9 +11174,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10796,7 +11184,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="19">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10810,7 +11210,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10820,7 +11220,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10834,17 +11234,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="colorScale" priority="124">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="125">
+    <cfRule type="dataBar" priority="126">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10856,9 +11246,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="colorScale" priority="122">
+    <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10868,7 +11256,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="123">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="dataBar" priority="124">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10880,9 +11270,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="colorScale" priority="120">
+    <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10892,7 +11280,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="121">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="dataBar" priority="122">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10904,9 +11294,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="colorScale" priority="118">
+    <cfRule type="colorScale" priority="121">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10916,7 +11304,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="119">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="dataBar" priority="120">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10928,9 +11318,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="colorScale" priority="116">
+    <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10940,7 +11328,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="117">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="dataBar" priority="118">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10952,9 +11342,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="colorScale" priority="114">
+    <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10964,7 +11352,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="115">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="dataBar" priority="116">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10976,9 +11366,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="colorScale" priority="112">
+    <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10988,7 +11376,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="113">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="colorScale" priority="113">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="114">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11002,7 +11402,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="colorScale" priority="110">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11012,7 +11412,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="111">
+    <cfRule type="dataBar" priority="112">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11026,7 +11426,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48">
-    <cfRule type="colorScale" priority="108">
+    <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11036,7 +11436,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="109">
+    <cfRule type="dataBar" priority="110">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11050,7 +11450,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49">
-    <cfRule type="colorScale" priority="106">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11060,7 +11460,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="107">
+    <cfRule type="dataBar" priority="108">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11074,7 +11474,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="colorScale" priority="104">
+    <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11084,7 +11484,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="105">
+    <cfRule type="dataBar" priority="106">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11098,7 +11498,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="colorScale" priority="102">
+    <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11108,7 +11508,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="103">
+    <cfRule type="dataBar" priority="104">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11122,17 +11522,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="colorScale" priority="100">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="101">
+    <cfRule type="dataBar" priority="102">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11144,9 +11534,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="colorScale" priority="98">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11156,7 +11544,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="99">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="dataBar" priority="100">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11168,9 +11558,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11180,7 +11568,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="9">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11192,9 +11582,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="colorScale" priority="96">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11204,7 +11592,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="97">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="colorScale" priority="97">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="98">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11218,17 +11618,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="colorScale" priority="94">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="95">
+    <cfRule type="dataBar" priority="96">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11240,9 +11630,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="colorScale" priority="92">
+    <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11252,7 +11640,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="93">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="dataBar" priority="94">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11264,9 +11654,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="colorScale" priority="90">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11276,7 +11664,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="91">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="dataBar" priority="92">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11288,9 +11678,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="colorScale" priority="88">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11300,7 +11688,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="89">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="dataBar" priority="90">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11312,9 +11702,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="colorScale" priority="86">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11324,7 +11712,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="87">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="dataBar" priority="88">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11336,9 +11726,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11348,7 +11736,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="85">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="dataBar" priority="86">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11360,9 +11750,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11372,7 +11760,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="21">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11386,7 +11786,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="colorScale" priority="82">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11396,7 +11796,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="83">
+    <cfRule type="dataBar" priority="84">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11410,7 +11810,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64">
-    <cfRule type="colorScale" priority="80">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11420,7 +11820,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="81">
+    <cfRule type="dataBar" priority="82">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11434,17 +11834,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="colorScale" priority="78">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="79">
+    <cfRule type="dataBar" priority="80">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11456,9 +11846,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="colorScale" priority="76">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11468,7 +11856,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="77">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule type="dataBar" priority="78">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11480,9 +11870,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="colorScale" priority="74">
+    <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11492,7 +11880,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="75">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="dataBar" priority="76">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11504,9 +11894,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="colorScale" priority="72">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11516,7 +11904,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="73">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="dataBar" priority="74">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11528,9 +11918,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11540,7 +11928,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="71">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69">
+    <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11552,9 +11942,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11564,7 +11952,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="69">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D70">
+    <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11576,9 +11966,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11588,7 +11976,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="67">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="dataBar" priority="68">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11600,9 +11990,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
-    <cfRule type="colorScale" priority="64">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11612,7 +12000,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="65">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D72">
+    <cfRule type="dataBar" priority="66">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11624,9 +12014,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
-    <cfRule type="colorScale" priority="62">
+    <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11636,7 +12024,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="63">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D73">
+    <cfRule type="dataBar" priority="64">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11648,9 +12038,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
-    <cfRule type="colorScale" priority="60">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11660,7 +12048,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="61">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D74">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="62">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11674,17 +12074,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="colorScale" priority="58">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="59">
+    <cfRule type="dataBar" priority="60">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11696,9 +12086,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D76">
-    <cfRule type="colorScale" priority="56">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11708,7 +12096,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="57">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D76">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="58">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11722,7 +12122,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11732,7 +12132,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="55">
+    <cfRule type="dataBar" priority="56">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11746,17 +12146,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="53">
+    <cfRule type="dataBar" priority="54">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11768,9 +12158,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D79">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11780,7 +12168,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="51">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D79">
+    <cfRule type="dataBar" priority="52">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11792,9 +12182,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D80">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11804,7 +12192,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="49">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D80">
+    <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11816,9 +12206,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D81">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11828,7 +12216,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="47">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D81">
+    <cfRule type="dataBar" priority="48">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11840,9 +12230,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D82">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11852,7 +12240,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="39">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D82">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11866,7 +12266,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11876,7 +12276,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11890,17 +12290,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="38">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11912,9 +12302,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11924,7 +12312,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="35">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D85">
+    <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11936,9 +12326,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D86">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11948,7 +12336,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="15">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D86">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11962,17 +12362,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11984,9 +12374,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D88">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11996,7 +12384,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="29">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D88">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -12010,7 +12410,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12020,7 +12420,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="27">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -12034,7 +12434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D90">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12044,7 +12444,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -12058,7 +12458,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12070,7 +12470,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12082,7 +12482,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T91:T97 S87:S90 S63:S82 S40:S53 S84:S85 S36:S37 S55:S61 S2:S3 S14:S34 S9:S12 S6">
-    <cfRule type="colorScale" priority="205">
+    <cfRule type="colorScale" priority="206">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y1:Y1048576">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>